<commit_message>
Clean and compile data
</commit_message>
<xml_diff>
--- a/Raw_Data/2023_Raw_Seine_Data.xlsx
+++ b/Raw_Data/2023_Raw_Seine_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klankowicz\Documents\GitHub\CBASS\Raw_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7331B6-A3D6-4C3E-B200-C5FB28229649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51379B64-261C-483C-B346-54E80ECFF143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{DCFEE481-2F8A-4B90-97BA-79BA2E708FE8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{DCFEE481-2F8A-4B90-97BA-79BA2E708FE8}"/>
   </bookViews>
   <sheets>
     <sheet name="sites" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5133" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5132" uniqueCount="203">
   <si>
     <t>site_name</t>
   </si>
@@ -596,9 +596,6 @@
     <t>thousands of alewife escaping net</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -2774,7 +2771,7 @@
         <v>152</v>
       </c>
       <c r="K40" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
@@ -2800,7 +2797,7 @@
         <v>151</v>
       </c>
       <c r="K41" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
@@ -2826,7 +2823,7 @@
         <v>151</v>
       </c>
       <c r="K42" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
@@ -2895,7 +2892,7 @@
         <v>171</v>
       </c>
       <c r="K45" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
@@ -2967,7 +2964,7 @@
         <v>152</v>
       </c>
       <c r="K48" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
@@ -2990,10 +2987,10 @@
         <v>151</v>
       </c>
       <c r="J49" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K49" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
@@ -3019,7 +3016,7 @@
         <v>152</v>
       </c>
       <c r="K50" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
@@ -3071,7 +3068,7 @@
         <v>178</v>
       </c>
       <c r="K52" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
@@ -3097,7 +3094,7 @@
         <v>152</v>
       </c>
       <c r="K53" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
@@ -3123,7 +3120,7 @@
         <v>152</v>
       </c>
       <c r="K54" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
@@ -3195,7 +3192,7 @@
         <v>151</v>
       </c>
       <c r="K57" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.3">
@@ -3264,7 +3261,7 @@
         <v>152</v>
       </c>
       <c r="K60" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
@@ -3336,7 +3333,7 @@
         <v>152</v>
       </c>
       <c r="K63" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
@@ -3385,7 +3382,7 @@
         <v>151</v>
       </c>
       <c r="K65" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
@@ -3549,7 +3546,7 @@
         <v>152</v>
       </c>
       <c r="K72" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.3">
@@ -3667,7 +3664,7 @@
         <v>151</v>
       </c>
       <c r="K77" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.3">
@@ -3726,7 +3723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{658F56C7-EABB-448F-A9D6-991BE28016FF}">
   <dimension ref="A1:F1841"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A352" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C1842" sqref="C1842"/>
     </sheetView>
@@ -11974,7 +11971,7 @@
         <v>36</v>
       </c>
       <c r="E539" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="540" spans="1:5" x14ac:dyDescent="0.3">
@@ -11988,7 +11985,7 @@
         <v>36</v>
       </c>
       <c r="E540" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="541" spans="1:5" x14ac:dyDescent="0.3">
@@ -12002,7 +11999,7 @@
         <v>36</v>
       </c>
       <c r="E541" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="542" spans="1:5" x14ac:dyDescent="0.3">
@@ -12016,7 +12013,7 @@
         <v>36</v>
       </c>
       <c r="E542" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="543" spans="1:5" x14ac:dyDescent="0.3">
@@ -12030,7 +12027,7 @@
         <v>36</v>
       </c>
       <c r="E543" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="544" spans="1:5" x14ac:dyDescent="0.3">
@@ -12044,7 +12041,7 @@
         <v>36</v>
       </c>
       <c r="E544" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="545" spans="1:5" x14ac:dyDescent="0.3">
@@ -12126,7 +12123,7 @@
         <v>36</v>
       </c>
       <c r="E549" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="550" spans="1:5" x14ac:dyDescent="0.3">
@@ -12140,7 +12137,7 @@
         <v>36</v>
       </c>
       <c r="E550" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="551" spans="1:5" x14ac:dyDescent="0.3">
@@ -12154,7 +12151,7 @@
         <v>36</v>
       </c>
       <c r="E551" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="552" spans="1:5" x14ac:dyDescent="0.3">
@@ -12168,7 +12165,7 @@
         <v>36</v>
       </c>
       <c r="E552" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="553" spans="1:5" x14ac:dyDescent="0.3">
@@ -12182,7 +12179,7 @@
         <v>36</v>
       </c>
       <c r="E553" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="554" spans="1:5" x14ac:dyDescent="0.3">
@@ -12196,7 +12193,7 @@
         <v>36</v>
       </c>
       <c r="E554" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="555" spans="1:5" x14ac:dyDescent="0.3">
@@ -12210,7 +12207,7 @@
         <v>36</v>
       </c>
       <c r="E555" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="556" spans="1:5" x14ac:dyDescent="0.3">
@@ -12224,7 +12221,7 @@
         <v>36</v>
       </c>
       <c r="E556" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="557" spans="1:5" x14ac:dyDescent="0.3">
@@ -12238,7 +12235,7 @@
         <v>36</v>
       </c>
       <c r="E557" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="558" spans="1:5" x14ac:dyDescent="0.3">
@@ -12252,7 +12249,7 @@
         <v>36</v>
       </c>
       <c r="E558" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="559" spans="1:5" x14ac:dyDescent="0.3">
@@ -12266,7 +12263,7 @@
         <v>36</v>
       </c>
       <c r="E559" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="560" spans="1:5" x14ac:dyDescent="0.3">
@@ -12280,7 +12277,7 @@
         <v>36</v>
       </c>
       <c r="E560" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="561" spans="1:5" x14ac:dyDescent="0.3">
@@ -12294,7 +12291,7 @@
         <v>36</v>
       </c>
       <c r="E561" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="562" spans="1:5" x14ac:dyDescent="0.3">
@@ -12339,7 +12336,7 @@
         <v>36</v>
       </c>
       <c r="E564" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="565" spans="1:5" x14ac:dyDescent="0.3">
@@ -12353,7 +12350,7 @@
         <v>36</v>
       </c>
       <c r="E565" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="566" spans="1:5" x14ac:dyDescent="0.3">
@@ -13774,7 +13771,7 @@
         <v>7</v>
       </c>
       <c r="C659" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E659">
         <v>54</v>
@@ -14183,7 +14180,7 @@
         <v>36</v>
       </c>
       <c r="E688" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="689" spans="1:5" x14ac:dyDescent="0.3">
@@ -14197,7 +14194,7 @@
         <v>36</v>
       </c>
       <c r="E689" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="690" spans="1:5" x14ac:dyDescent="0.3">
@@ -14211,7 +14208,7 @@
         <v>36</v>
       </c>
       <c r="E690" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="691" spans="1:5" x14ac:dyDescent="0.3">
@@ -14225,7 +14222,7 @@
         <v>36</v>
       </c>
       <c r="E691" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="692" spans="1:5" x14ac:dyDescent="0.3">
@@ -14239,7 +14236,7 @@
         <v>36</v>
       </c>
       <c r="E692" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="693" spans="1:5" x14ac:dyDescent="0.3">
@@ -14253,7 +14250,7 @@
         <v>36</v>
       </c>
       <c r="E693" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="694" spans="1:5" x14ac:dyDescent="0.3">
@@ -14267,7 +14264,7 @@
         <v>36</v>
       </c>
       <c r="E694" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="695" spans="1:5" x14ac:dyDescent="0.3">
@@ -14281,7 +14278,7 @@
         <v>36</v>
       </c>
       <c r="E695" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="696" spans="1:5" x14ac:dyDescent="0.3">
@@ -14295,7 +14292,7 @@
         <v>36</v>
       </c>
       <c r="E696" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="697" spans="1:5" x14ac:dyDescent="0.3">
@@ -14309,7 +14306,7 @@
         <v>36</v>
       </c>
       <c r="E697" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="698" spans="1:5" x14ac:dyDescent="0.3">
@@ -14323,7 +14320,7 @@
         <v>36</v>
       </c>
       <c r="E698" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="699" spans="1:5" x14ac:dyDescent="0.3">
@@ -14337,7 +14334,7 @@
         <v>36</v>
       </c>
       <c r="E699" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="700" spans="1:5" x14ac:dyDescent="0.3">
@@ -14351,7 +14348,7 @@
         <v>36</v>
       </c>
       <c r="E700" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="701" spans="1:5" x14ac:dyDescent="0.3">
@@ -14365,7 +14362,7 @@
         <v>36</v>
       </c>
       <c r="E701" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="702" spans="1:5" x14ac:dyDescent="0.3">
@@ -16223,7 +16220,7 @@
         <v>14</v>
       </c>
       <c r="C832" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E832">
         <v>44</v>
@@ -16237,7 +16234,7 @@
         <v>14</v>
       </c>
       <c r="C833" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E833">
         <v>46</v>
@@ -16251,7 +16248,7 @@
         <v>14</v>
       </c>
       <c r="C834" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E834">
         <v>42</v>
@@ -16265,7 +16262,7 @@
         <v>14</v>
       </c>
       <c r="C835" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E835">
         <v>40</v>
@@ -16279,7 +16276,7 @@
         <v>14</v>
       </c>
       <c r="C836" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E836">
         <v>45</v>
@@ -16293,7 +16290,7 @@
         <v>14</v>
       </c>
       <c r="C837" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E837">
         <v>47</v>
@@ -16307,7 +16304,7 @@
         <v>14</v>
       </c>
       <c r="C838" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E838">
         <v>48</v>
@@ -16321,7 +16318,7 @@
         <v>14</v>
       </c>
       <c r="C839" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E839">
         <v>48</v>
@@ -16335,7 +16332,7 @@
         <v>14</v>
       </c>
       <c r="C840" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E840">
         <v>42</v>
@@ -16349,7 +16346,7 @@
         <v>14</v>
       </c>
       <c r="C841" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E841">
         <v>47</v>
@@ -16363,7 +16360,7 @@
         <v>14</v>
       </c>
       <c r="C842" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E842">
         <v>47</v>
@@ -16377,7 +16374,7 @@
         <v>14</v>
       </c>
       <c r="C843" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E843">
         <v>44</v>
@@ -16391,7 +16388,7 @@
         <v>14</v>
       </c>
       <c r="C844" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E844">
         <v>44</v>
@@ -16405,7 +16402,7 @@
         <v>14</v>
       </c>
       <c r="C845" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E845">
         <v>43</v>
@@ -16419,7 +16416,7 @@
         <v>14</v>
       </c>
       <c r="C846" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E846">
         <v>63</v>
@@ -16433,7 +16430,7 @@
         <v>14</v>
       </c>
       <c r="C847" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E847">
         <v>42</v>
@@ -16447,7 +16444,7 @@
         <v>14</v>
       </c>
       <c r="C848" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E848">
         <v>44</v>
@@ -16461,7 +16458,7 @@
         <v>14</v>
       </c>
       <c r="C849" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E849">
         <v>44</v>
@@ -16475,7 +16472,7 @@
         <v>14</v>
       </c>
       <c r="C850" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E850">
         <v>45</v>
@@ -16489,7 +16486,7 @@
         <v>14</v>
       </c>
       <c r="C851" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E851">
         <v>43</v>
@@ -16503,7 +16500,7 @@
         <v>14</v>
       </c>
       <c r="C852" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E852">
         <v>37</v>
@@ -16517,7 +16514,7 @@
         <v>14</v>
       </c>
       <c r="C853" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E853">
         <v>42</v>
@@ -16531,7 +16528,7 @@
         <v>14</v>
       </c>
       <c r="C854" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E854">
         <v>47</v>
@@ -16545,7 +16542,7 @@
         <v>14</v>
       </c>
       <c r="C855" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E855">
         <v>44</v>
@@ -16559,7 +16556,7 @@
         <v>14</v>
       </c>
       <c r="C856" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E856">
         <v>49</v>
@@ -17061,7 +17058,7 @@
         <v>14</v>
       </c>
       <c r="C891" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E891">
         <v>89</v>
@@ -19198,7 +19195,7 @@
         <v>36</v>
       </c>
       <c r="E1037" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="1038" spans="1:5" x14ac:dyDescent="0.3">
@@ -19212,7 +19209,7 @@
         <v>36</v>
       </c>
       <c r="E1038" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="1039" spans="1:5" x14ac:dyDescent="0.3">
@@ -19226,7 +19223,7 @@
         <v>36</v>
       </c>
       <c r="E1039" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="1040" spans="1:5" x14ac:dyDescent="0.3">
@@ -19240,7 +19237,7 @@
         <v>36</v>
       </c>
       <c r="E1040" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="1041" spans="1:5" x14ac:dyDescent="0.3">
@@ -19254,7 +19251,7 @@
         <v>36</v>
       </c>
       <c r="E1041" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="1042" spans="1:5" x14ac:dyDescent="0.3">
@@ -19268,7 +19265,7 @@
         <v>36</v>
       </c>
       <c r="E1042" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="1043" spans="1:5" x14ac:dyDescent="0.3">
@@ -19282,7 +19279,7 @@
         <v>36</v>
       </c>
       <c r="E1043" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="1044" spans="1:5" x14ac:dyDescent="0.3">
@@ -26585,7 +26582,7 @@
         <v>14</v>
       </c>
       <c r="C1546" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E1546">
         <v>210</v>
@@ -30923,9 +30920,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6954D5E-4D80-497F-8F08-8B5E5FFD78C8}">
   <dimension ref="A1:D219"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32249,8 +32246,8 @@
       <c r="C94" t="s">
         <v>36</v>
       </c>
-      <c r="D94" t="s">
-        <v>183</v>
+      <c r="D94">
+        <v>38</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
@@ -32541,7 +32538,7 @@
         <v>7</v>
       </c>
       <c r="C115" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D115">
         <v>1</v>
@@ -32723,7 +32720,7 @@
         <v>14</v>
       </c>
       <c r="C128" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D128">
         <v>130</v>
@@ -32807,7 +32804,7 @@
         <v>14</v>
       </c>
       <c r="C134" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D134">
         <v>1</v>
@@ -33647,7 +33644,7 @@
         <v>14</v>
       </c>
       <c r="C194" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D194">
         <v>1</v>

</xml_diff>